<commit_message>
Fixed some text and chart
</commit_message>
<xml_diff>
--- a/data/experiment-results/free_field_of_antenna_6-14GHz_0-6dBm_generator_output_distance_5mm.xlsx
+++ b/data/experiment-results/free_field_of_antenna_6-14GHz_0-6dBm_generator_output_distance_5mm.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Frequency (GHz)</t>
   </si>
@@ -33,6 +33,18 @@
   <si>
     <t xml:space="preserve">6 dBm</t>
   </si>
+  <si>
+    <t xml:space="preserve">8 GHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 GHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 GHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power</t>
+  </si>
 </sst>
 </file>
 
@@ -41,7 +53,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -79,6 +91,16 @@
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -218,10 +240,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0774090395039582"/>
-          <c:y val="0.0444519621109608"/>
-          <c:w val="0.883671957259291"/>
-          <c:h val="0.801826792963464"/>
+          <c:x val="0.077418096723869"/>
+          <c:y val="0.0444609866684713"/>
+          <c:w val="0.883541341653666"/>
+          <c:h val="0.801583541990932"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -710,11 +732,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="6581667"/>
-        <c:axId val="5470400"/>
+        <c:axId val="20513251"/>
+        <c:axId val="56359664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="6581667"/>
+        <c:axId val="20513251"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="14"/>
@@ -781,12 +803,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5470400"/>
+        <c:crossAx val="56359664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="5470400"/>
+        <c:axId val="56359664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -852,7 +874,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6581667"/>
+        <c:crossAx val="20513251"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -913,20 +935,517 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0733089227211409"/>
+          <c:y val="0.0332319134550372"/>
+          <c:w val="0.892734630950087"/>
+          <c:h val="0.82657200811359"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lvtemporary_573329!$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8 GHz</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="18360">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>lvtemporary_573329!$B$11:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>lvtemporary_573329!$B$4:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.091222</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.39271</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.71476</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lvtemporary_573329!$E$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>11 GHz</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff4000"/>
+            </a:solidFill>
+            <a:ln w="18360">
+              <a:solidFill>
+                <a:srgbClr val="ff4000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff4000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>lvtemporary_573329!$B$11:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>lvtemporary_573329!$B$7:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.38203</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.81182</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3952</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lvtemporary_573329!$E$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>12 GHz</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="43c330"/>
+            </a:solidFill>
+            <a:ln w="18360">
+              <a:solidFill>
+                <a:srgbClr val="43c330"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="43c330"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>lvtemporary_573329!$B$11:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>lvtemporary_573329!$B$8:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.24589</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.50181</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.97653</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="27448492"/>
+        <c:axId val="67199722"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="27448492"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="6"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1200" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1200" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Power (dBm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="67199722"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="3"/>
+        <c:minorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="67199722"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1200" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1200" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Intensity (a.u.)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="27448492"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.111804832928662"/>
+          <c:y val="0.0642239048134127"/>
+          <c:w val="0.117817088680772"/>
+          <c:h val="0.138250405624662"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1200" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>369720</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>128520</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>9000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>685440</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>114840</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>323640</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>175680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -934,12 +1453,42 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4233240" y="1271520"/>
-        <a:ext cx="9231120" cy="5320440"/>
+        <a:off x="14159520" y="0"/>
+        <a:ext cx="9230040" cy="5319360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>595080</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>334080</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>180720</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="4458600" y="0"/>
+        <a:ext cx="9340200" cy="5324400"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -953,10 +1502,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T26" activeCellId="0" sqref="T26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC37" activeCellId="0" sqref="AC37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1021,6 +1570,9 @@
       <c r="D4" s="1" t="n">
         <v>1.71476</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -1063,6 +1615,9 @@
       <c r="D7" s="1" t="n">
         <v>4.3952</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -1077,6 +1632,9 @@
       <c r="D8" s="1" t="n">
         <v>3.97653</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -1104,6 +1662,20 @@
       </c>
       <c r="D10" s="1" t="n">
         <v>4.49072</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>